<commit_message>
transaction data basic import final
</commit_message>
<xml_diff>
--- a/coreapi/coreapi/v0/ui/campaign/Campaign Data.xlsx
+++ b/coreapi/coreapi/v0/ui/campaign/Campaign Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Start Date</t>
   </si>
@@ -49,49 +49,7 @@
     <t xml:space="preserve">Supplier Id</t>
   </si>
   <si>
-    <t xml:space="preserve">poster count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poster Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poster Days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standee count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standee Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standee Days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flier Frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flier Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flier Days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stall count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stall price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No of stall days </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gateway Arch Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gateway Arch Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. Gateway Arch Days</t>
+    <t xml:space="preserve">total_negotiated_price</t>
   </si>
   <si>
     <t xml:space="preserve">NOINO50RSATG</t>
@@ -185,7 +143,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,10 +154,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -223,10 +177,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,16 +191,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="19" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="17.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,54 +234,12 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="0" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="3" t="n">
         <v>43314</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="3" t="n">
         <v>43316</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -349,53 +261,17 @@
         <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="W2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="X2" s="0" t="n">
-        <v>3</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="3" t="n">
         <v>43314</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="3" t="n">
         <v>43316</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -417,46 +293,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>3</v>
+        <v>4500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>